<commit_message>
Merged PR 9239: Tests fix
Tests fix
</commit_message>
<xml_diff>
--- a/Source/Tam/MaestroTests/SupportTests/Services.Broadcast.IntegrationTests/Files/Vpvh/VPVH_valid.xlsx
+++ b/Source/Tam/MaestroTests/SupportTests/Services.Broadcast.IntegrationTests/Files/Vpvh/VPVH_valid.xlsx
@@ -1,32 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephanwhyte/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\sroibu\Source\Repos\Broadcast\Source\Tam\MaestroTests\SupportTests\Services.Broadcast.IntegrationTests\Files\Vpvh\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69820564-B530-5643-BBC5-8C0E6090020B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{1CF935C8-14ED-4EF3-882E-6F1BAB940CF6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7080" yWindow="1840" windowWidth="25240" windowHeight="12760" xr2:uid="{A2A540DF-33A0-B04B-BFBF-AABE6FC8DEB0}"/>
+    <workbookView xWindow="7080" yWindow="1845" windowWidth="25245" windowHeight="12765" xr2:uid="{A2A540DF-33A0-B04B-BFBF-AABE6FC8DEB0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" calcOnSave="0"/>
+  <calcPr calcId="179017" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -467,12 +459,12 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -489,7 +481,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -506,7 +498,7 @@
         <v>0.69</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -523,7 +515,7 @@
         <v>8.3000000000000004E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -540,7 +532,7 @@
         <v>0.22700000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -557,7 +549,7 @@
         <v>0.27800000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -574,7 +566,7 @@
         <v>0.38100000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -591,7 +583,7 @@
         <v>0.39</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -608,7 +600,7 @@
         <v>0.47099999999999997</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -625,7 +617,7 @@
         <v>6.5000000000000002E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -642,7 +634,7 @@
         <v>0.16600000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -659,7 +651,7 @@
         <v>0.20300000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -676,7 +668,7 @@
         <v>0.27900000000000003</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -684,7 +676,7 @@
         <v>0</v>
       </c>
       <c r="C13" s="4">
-        <v>0.28599999999999998</v>
+        <v>0.28499999999999998</v>
       </c>
       <c r="D13" s="4">
         <v>0.34499999999999997</v>

</xml_diff>

<commit_message>
Merged PR 9273: Unit tests
Unit tests for BusinessEngines and Extensions on Services.Broadcast
</commit_message>
<xml_diff>
--- a/Source/Tam/MaestroTests/SupportTests/Services.Broadcast.IntegrationTests/Files/Vpvh/VPVH_valid.xlsx
+++ b/Source/Tam/MaestroTests/SupportTests/Services.Broadcast.IntegrationTests/Files/Vpvh/VPVH_valid.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\sroibu\Source\Repos\Broadcast\Source\Tam\MaestroTests\SupportTests\Services.Broadcast.IntegrationTests\Files\Vpvh\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\irozani\Broadcast\Source\Tam\MaestroTests\SupportTests\Services.Broadcast.IntegrationTests\Files\Vpvh\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{1CF935C8-14ED-4EF3-882E-6F1BAB940CF6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{FD5F8A11-5143-4FF9-B7A5-C18F6C04CCEB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7080" yWindow="1845" windowWidth="25245" windowHeight="12765" xr2:uid="{A2A540DF-33A0-B04B-BFBF-AABE6FC8DEB0}"/>
   </bookViews>
@@ -459,7 +459,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -676,13 +676,13 @@
         <v>0</v>
       </c>
       <c r="C13" s="4">
-        <v>0.28499999999999998</v>
+        <v>0.28599999999999998</v>
       </c>
       <c r="D13" s="4">
         <v>0.34499999999999997</v>
       </c>
       <c r="E13" s="4">
-        <v>0.249</v>
+        <v>0.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>